<commit_message>
Final publication; add copyright.
</commit_message>
<xml_diff>
--- a/dev-topics-algorithms/dev-topics-nasa-sensor/documentation/concepts.xlsx
+++ b/dev-topics-algorithms/dev-topics-nasa-sensor/documentation/concepts.xlsx
@@ -913,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="26"/>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="30"/>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="30"/>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="30"/>
       <c r="D26" s="14"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
       <c r="G26" s="30"/>
       <c r="H26" s="31"/>
       <c r="J26" t="s">
@@ -1146,7 +1146,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="30"/>
@@ -1158,19 +1158,23 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>5</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="17">
+        <v>3</v>
+      </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="30"/>
       <c r="H28" s="31"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="42"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" s="32"/>
       <c r="C29" s="11"/>
@@ -1181,94 +1185,78 @@
       <c r="F29" s="15"/>
       <c r="G29" s="30"/>
       <c r="H29" s="31"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="42"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>3</v>
-      </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="17">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="30"/>
       <c r="H30" s="31"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="44"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="30"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="31"/>
+      <c r="F31" s="18">
+        <v>2</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37">
+        <v>2</v>
+      </c>
+      <c r="G32" s="38"/>
+      <c r="H32" s="39"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
         <v>1</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="18">
+      <c r="D33">
         <v>2</v>
       </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="33"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>0</v>
-      </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37">
-        <v>2</v>
-      </c>
-      <c r="G33" s="38"/>
-      <c r="H33" s="39"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34">
+      <c r="E33">
         <v>3</v>
       </c>
-      <c r="F34">
+      <c r="F33">
         <v>4</v>
       </c>
-      <c r="G34">
+      <c r="G33">
         <v>5</v>
       </c>
-      <c r="H34">
+      <c r="H33">
         <v>6</v>
       </c>
-      <c r="I34">
+      <c r="I33">
         <v>7</v>
       </c>
-      <c r="J34">
+      <c r="J33">
         <v>8</v>
       </c>
-      <c r="K34">
+      <c r="K33">
         <v>9</v>
       </c>
     </row>

</xml_diff>